<commit_message>
feat: dark mode, user-spanish things, configuration's pipeline forms and format, tools to db-json-ify configs
</commit_message>
<xml_diff>
--- a/data/database/pipelines.xlsx
+++ b/data/database/pipelines.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2026-01-30 17:07:43</t>
+          <t>2026-01-30 20:30:28</t>
         </is>
       </c>
     </row>
@@ -531,12 +531,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SIMCE Lenguaje (Copia)</t>
+          <t>Proceso de prueba</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Workflow SIMCE</t>
+          <t>Testing pipeline</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>EXCEL</t>
+          <t>PDF</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>

</xml_diff>